<commit_message>
done student list with export and refresh button
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -12,7 +12,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Number of Borrowed Books</t>
+  </si>
   <si>
     <t>a123456</t>
   </si>
@@ -134,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -156,25 +174,25 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="n" s="0">
-        <v>2.0</v>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>2.0</v>
@@ -182,19 +200,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>2.0</v>
@@ -202,19 +220,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>2.0</v>
@@ -222,41 +240,61 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="F7" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added search button in StudentListPanel when student is clicked in the table may new window mag papakita ng mga borrowed books when student is clicked auto copy ang student ID later gagamitin para sa return books
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Student ID</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Number of Borrowed Books</t>
+    <t>Borrowed Books</t>
   </si>
   <si>
     <t>a123456</t>
@@ -57,6 +57,33 @@
   </si>
   <si>
     <t>098765432</t>
+  </si>
+  <si>
+    <t>a32132111231</t>
+  </si>
+  <si>
+    <t>sadadasd</t>
+  </si>
+  <si>
+    <t>HSU</t>
+  </si>
+  <si>
+    <t>sadad</t>
+  </si>
+  <si>
+    <t>321313123313</t>
+  </si>
+  <si>
+    <t>a342423244</t>
+  </si>
+  <si>
+    <t>sdaasdsadasdsa</t>
+  </si>
+  <si>
+    <t>tcsada</t>
+  </si>
+  <si>
+    <t>321313131212</t>
   </si>
   <si>
     <t>a55664478</t>
@@ -152,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,7 +222,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -215,7 +242,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -235,7 +262,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -249,30 +276,30 @@
         <v>8</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>1.0</v>
@@ -280,21 +307,61 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s" s="0">
         <v>31</v>
       </c>
       <c r="F7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F9" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added export date, buttons design
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+  <si>
+    <t>Export Date and Time: 2024-05-29 13:12:22</t>
+  </si>
   <si>
     <t>Student ID</t>
   </si>
@@ -120,6 +123,15 @@
   </si>
   <si>
     <t>0987323145</t>
+  </si>
+  <si>
+    <t>a78777882</t>
+  </si>
+  <si>
+    <t>Michael Jackstone</t>
+  </si>
+  <si>
+    <t>09887665432</t>
   </si>
   <si>
     <t>b123456</t>
@@ -142,13 +154,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,115 +193,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B3" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="C3" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="D3" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="E3" t="s" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+      <c r="F3" t="s" s="1">
         <v>6</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>1.0</v>
@@ -287,19 +256,19 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>1.0</v>
@@ -307,19 +276,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>1.0</v>
@@ -327,19 +296,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F8" t="n" s="0">
         <v>1.0</v>
@@ -347,21 +316,101 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="F11" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="B12" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="C12" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="E9" t="s" s="0">
+      <c r="F12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="F9" t="n" s="0">
+      <c r="B13" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F13" t="n" s="0">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>